<commit_message>
Spring Data JPA with Spring Boot And Hibernate
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Desktop\Cognizant-Digital-Nurture-4.0-JFSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416DA72B-212B-4F67-8FA4-317AB9DF88C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6BE4B6-7CC7-40EB-AD21-D1D2AE198D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -470,24 +468,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -502,15 +486,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,8 +851,8 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11:F12"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,28 +865,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1055,30 +1053,30 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11" s="17">
         <v>2</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>3</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="26" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="16"/>
@@ -1142,65 +1140,65 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="7">
         <v>1</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="7">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="7">
         <v>2</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4" t="s">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="7">
         <v>3</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="7">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4" t="s">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1437,19 +1435,19 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
+      <c r="A31" s="19">
         <v>5</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="19">
         <v>1</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="19" t="s">
         <v>62</v>
       </c>
       <c r="F31" s="15" t="s">
@@ -1460,11 +1458,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="16"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="16"/>
       <c r="G32" s="6" t="s">
         <v>64</v>
@@ -1789,11 +1787,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
@@ -1806,12 +1799,26 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2071,15 +2078,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2092,6 +2090,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2107,14 +2113,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Week 4 Spring security and JWT
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Desktop\Cognizant-Digital-Nurture-4.0-JFSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6BE4B6-7CC7-40EB-AD21-D1D2AE198D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182F9C96-D840-4B92-8D0D-DDD92F4CB873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -474,28 +474,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,11 +494,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,8 +851,8 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,28 +865,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="22"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1053,34 +1053,34 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="A11" s="19">
         <v>2</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="19">
         <v>3</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
@@ -1203,116 +1203,116 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="7">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="7">
         <v>1</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="7">
         <v>3</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="7">
         <v>2</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="7">
         <v>3</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="7">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="7">
         <v>3</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="7">
         <v>3</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1435,22 +1435,22 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="19">
+      <c r="A31" s="11">
         <v>5</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="11">
         <v>1</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="13" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="5" t="s">
@@ -1458,12 +1458,12 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="16"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="6" t="s">
         <v>64</v>
       </c>
@@ -1787,6 +1787,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
@@ -1803,22 +1804,12 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2078,6 +2069,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2090,14 +2090,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2113,6 +2105,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>